<commit_message>
adding departements n filieres
</commit_message>
<xml_diff>
--- a/soutenances.xlsx
+++ b/soutenances.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asus\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asus\Desktop\AppSoutenance\Backend-GestionPFE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{304BE84E-50B7-46D9-8A8A-4FF0E3D771C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2514DAC-3CBA-41D0-ABA5-92F4D5D67C43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{EF6CCBB0-5ACF-472E-90E7-36E13B39463F}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>nom_etudiant</t>
   </si>
@@ -78,13 +78,25 @@
   </si>
   <si>
     <t>ali</t>
+  </si>
+  <si>
+    <t>test1</t>
+  </si>
+  <si>
+    <t>tes1t@gmail.com odoo</t>
+  </si>
+  <si>
+    <t>ahmed</t>
+  </si>
+  <si>
+    <t>mec</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -100,18 +112,55 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF444444"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFFFFFFF"/>
+      </left>
       <right/>
       <top/>
       <bottom/>
@@ -122,9 +171,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -440,10 +498,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2FE0014-0EFA-41AB-AA49-0DA545A65DE7}">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -456,7 +514,7 @@
     <col min="9" max="9" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -484,8 +542,13 @@
       <c r="I1" t="s">
         <v>8</v>
       </c>
+      <c r="J1" s="2"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -499,10 +562,29 @@
         <v>12</v>
       </c>
     </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="K1:N1"/>
+  </mergeCells>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{34B9FEAF-8260-4A45-B5A2-244829173C51}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{F6FC007C-1107-4E54-AA02-B9A0D7352211}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>